<commit_message>
Revised the overlap code. Instead of rotating slits about the center of the wafer, it offsets/translates them in the x and y directions. Found/realized that translating in the y direction is NOT NECESSARY. Will revert to previous commit and just modify the rotation calculation to be offset along x axis. Will make interpretation easier.
</commit_message>
<xml_diff>
--- a/overlap_calculation/slits_corner_coords.xlsx
+++ b/overlap_calculation/slits_corner_coords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkima\OneDrive\Documents\Demonpore\overlap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkima\OneDrive\Documents\Demonpore\Simulation\overlap_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:40009_{755CFA54-4C16-470C-BFBD-15970E20D75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{980E76CA-A49C-4821-91E3-5CEF276EB853}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:40009_{755CFA54-4C16-470C-BFBD-15970E20D75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13CE79A2-1AE2-44C9-B441-569AB3CF3C59}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revised the overlap code. Instead of rotating slits about the center of the wafer, it offsets/translates them in the x and y directions. Found/realized that translating in the y direction is NOT NECESSARY. Will revert to previous commit and just modify the rotation calculation to be offset along x axis. Will make interpretation easier."
This reverts commit 1bee24be97dd6dfc8f4b6a66ab47652684e80946.
</commit_message>
<xml_diff>
--- a/overlap_calculation/slits_corner_coords.xlsx
+++ b/overlap_calculation/slits_corner_coords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkima\OneDrive\Documents\Demonpore\Simulation\overlap_calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkima\OneDrive\Documents\Demonpore\overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:40009_{755CFA54-4C16-470C-BFBD-15970E20D75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13CE79A2-1AE2-44C9-B441-569AB3CF3C59}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:40009_{755CFA54-4C16-470C-BFBD-15970E20D75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{980E76CA-A49C-4821-91E3-5CEF276EB853}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>